<commit_message>
change voltage to 235
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8640" windowHeight="8184" activeTab="1"/>
+    <workbookView windowWidth="8867" windowHeight="5160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,30 +34,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -70,6 +55,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -78,16 +92,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,6 +130,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -132,6 +154,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -139,30 +169,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,14 +191,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -198,6 +198,24 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -213,7 +231,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,163 +375,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,6 +392,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,6 +443,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -445,24 +463,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -515,130 +515,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2363,500 +2363,747 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="12.8888888888889"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1">
-        <v>1135</v>
+        <v>291</v>
       </c>
       <c r="B1">
         <v>6930</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1">
+        <f>B1/A1</f>
+        <v>23.8144329896907</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
-        <v>1120</v>
+        <v>289</v>
       </c>
       <c r="B2">
-        <v>6684</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>6870</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C33" si="0">B2/A2</f>
+        <v>23.7716262975779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
-        <v>1079</v>
+        <v>288</v>
       </c>
       <c r="B3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>6870</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>23.8541666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
-        <v>1000</v>
+        <v>355</v>
       </c>
       <c r="B4">
-        <v>6277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>8566</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>24.1295774647887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
-        <v>1025</v>
+        <v>356</v>
       </c>
       <c r="B5">
-        <v>5957</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>8600</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>24.1573033707865</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
-        <v>1096</v>
+        <v>353</v>
       </c>
       <c r="B6">
-        <v>5834</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>8540</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>24.1926345609065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
-        <v>900</v>
+        <v>351</v>
       </c>
       <c r="B7">
-        <v>5638</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>8490</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>24.1880341880342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
-        <v>1000</v>
+        <v>351</v>
       </c>
       <c r="B8">
-        <v>5554</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>8460</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>24.1025641025641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
-        <v>1026</v>
+        <v>350</v>
       </c>
       <c r="B9">
-        <v>5533</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>8439</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>24.1114285714286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
-        <v>899</v>
+        <v>344</v>
       </c>
       <c r="B10">
-        <v>5427</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>8300</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>24.1279069767442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
-        <v>900</v>
+        <v>340</v>
       </c>
       <c r="B11">
-        <v>5314</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>8250</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>24.2647058823529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
-        <v>890</v>
+        <v>340</v>
       </c>
       <c r="B12">
-        <v>5295</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>8220</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>24.1764705882353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
-        <v>886</v>
+        <v>339</v>
       </c>
       <c r="B13">
-        <v>5085</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>8170</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>24.1002949852507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
-        <v>881</v>
+        <v>333</v>
       </c>
       <c r="B14">
-        <v>5059</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>8040</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>24.1441441441441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
-        <v>884</v>
+        <v>332</v>
       </c>
       <c r="B15">
-        <v>4638</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>8000</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>24.0963855421687</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
-        <v>880</v>
+        <v>331</v>
       </c>
       <c r="B16">
-        <v>4607</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>7970</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>24.0785498489426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
-        <v>876</v>
+        <v>330</v>
       </c>
       <c r="B17">
-        <v>4599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>7947</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>24.0818181818182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
-        <v>873</v>
+        <v>329</v>
       </c>
       <c r="B18">
-        <v>4585</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>7920</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>24.0729483282675</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
-        <v>862</v>
+        <v>326</v>
       </c>
       <c r="B19">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>7880</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>24.1717791411043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
-        <v>868</v>
+        <v>321</v>
       </c>
       <c r="B20">
-        <v>4550</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>7700</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>23.98753894081</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
-        <v>868</v>
+        <v>320</v>
       </c>
       <c r="B21">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>7676</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>23.9875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
-        <v>867</v>
+        <v>312</v>
       </c>
       <c r="B22">
-        <v>4530</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>7541</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>24.1698717948718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
-        <v>862</v>
+        <v>314</v>
       </c>
       <c r="B23">
-        <v>4520</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>7522</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>23.9554140127389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
-        <v>867</v>
+        <v>311</v>
       </c>
       <c r="B24">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>7470</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>24.0192926045016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
-        <v>856</v>
+        <v>309</v>
       </c>
       <c r="B25">
-        <v>4480</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>7426</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>24.0323624595469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
-        <v>848</v>
+        <v>308</v>
       </c>
       <c r="B26">
-        <v>4469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>7389</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>23.9902597402597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
-        <v>849</v>
+        <v>305</v>
       </c>
       <c r="B27">
-        <v>4465</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>7350</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>24.0983606557377</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
-        <v>846</v>
+        <v>293</v>
       </c>
       <c r="B28">
-        <v>4435</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>7020</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>23.9590443686007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
-        <v>850</v>
+        <v>127</v>
       </c>
       <c r="B29">
-        <v>4420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>2645</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>20.8267716535433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
-        <v>848</v>
+        <v>126</v>
       </c>
       <c r="B30">
-        <v>4410</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>2622</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>20.8095238095238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
-        <v>853</v>
+        <v>124</v>
       </c>
       <c r="B31">
-        <v>4395</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>2588</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>20.8709677419355</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
-        <v>841</v>
+        <v>122</v>
       </c>
       <c r="B32">
-        <v>4380</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>2524</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>20.6885245901639</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
-        <v>839</v>
+        <v>120</v>
       </c>
       <c r="B33">
-        <v>4370</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>2455</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>20.4583333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
-        <v>838</v>
+        <v>119</v>
       </c>
       <c r="B34">
-        <v>4355</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>2435</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:C61" si="1">B34/A34</f>
+        <v>20.4621848739496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
-        <v>838</v>
+        <v>117</v>
       </c>
       <c r="B35">
-        <v>4340</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>2390</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>20.4273504273504</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>836</v>
       </c>
       <c r="B36">
         <v>4325</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>5.17344497607655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>837</v>
       </c>
       <c r="B37">
         <v>4315</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>5.15531660692951</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>839</v>
       </c>
       <c r="B38">
         <v>4300</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>5.12514898688915</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>844</v>
       </c>
       <c r="B39">
         <v>4295</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>5.08886255924171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>842</v>
       </c>
       <c r="B40">
         <v>4270</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>5.07125890736342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>839</v>
       </c>
       <c r="B41">
         <v>4265</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>5.0834326579261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>857</v>
       </c>
       <c r="B42">
         <v>4260</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>4.9708284714119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>840</v>
       </c>
       <c r="B43">
         <v>4250</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>5.05952380952381</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>830</v>
       </c>
       <c r="B44">
         <v>4240</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>5.10843373493976</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>830</v>
       </c>
       <c r="B45">
         <v>4230</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>5.09638554216868</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>832</v>
       </c>
       <c r="B46">
         <v>4210</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>5.06009615384615</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>829</v>
       </c>
       <c r="B47">
         <v>4200</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>5.06634499396864</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>827</v>
       </c>
       <c r="B48">
         <v>4185</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>5.06045949214027</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>836</v>
       </c>
       <c r="B49">
         <v>4165</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>4.98205741626794</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>842</v>
       </c>
       <c r="B50">
         <v>4160</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>4.94061757719715</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>840</v>
       </c>
       <c r="B51">
         <v>4150</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>4.94047619047619</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>834</v>
       </c>
       <c r="B52">
         <v>4145</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>4.97002398081535</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>839</v>
       </c>
       <c r="B53">
         <v>4135</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>4.9284862932062</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>841</v>
       </c>
       <c r="B54">
         <v>4125</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>4.90487514863258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>828</v>
       </c>
       <c r="B55">
         <v>4120</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>4.97584541062802</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>184</v>
       </c>
       <c r="B56">
         <v>4060</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>22.0652173913043</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>184</v>
       </c>
       <c r="B57">
         <v>4050</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>22.0108695652174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>183</v>
       </c>
       <c r="B58">
         <v>4040</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>22.0765027322404</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>181</v>
       </c>
       <c r="B59">
         <v>4020</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>22.2099447513812</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>180</v>
       </c>
       <c r="B60">
         <v>4004</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>22.2444444444444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>180</v>
       </c>
       <c r="B61">
         <v>4000</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>22.2222222222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data for 10A
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8867" windowHeight="5160" activeTab="1"/>
+    <workbookView windowWidth="9515" windowHeight="6852" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -48,17 +48,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -68,36 +59,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,16 +72,47 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -133,7 +125,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -149,14 +149,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,15 +185,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,37 +201,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,7 +225,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +249,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,25 +303,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,7 +339,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,67 +375,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,26 +392,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -426,6 +406,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -445,6 +434,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -456,6 +454,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,18 +484,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,148 +497,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2363,747 +2363,1547 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="3" max="3" width="12.8888888888889"/>
+    <col min="3" max="4" width="12.8888888888889"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1">
-        <v>291</v>
+        <v>355</v>
       </c>
       <c r="B1">
-        <v>6930</v>
+        <v>8566</v>
       </c>
       <c r="C1">
-        <f>B1/A1</f>
-        <v>23.8144329896907</v>
+        <f t="shared" ref="C1:C25" si="0">B1/A1</f>
+        <v>24.1295774647887</v>
+      </c>
+      <c r="D1">
+        <f>AVERAGE(C1:C24)</f>
+        <v>24.1015477535835</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>289</v>
+        <v>356</v>
       </c>
       <c r="B2">
-        <v>6870</v>
+        <v>8600</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">B2/A2</f>
-        <v>23.7716262975779</v>
+        <f t="shared" si="0"/>
+        <v>24.1573033707865</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>288</v>
+        <v>353</v>
       </c>
       <c r="B3">
-        <v>6870</v>
+        <v>8540</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>23.8541666666667</v>
+        <v>24.1926345609065</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B4">
-        <v>8566</v>
+        <v>8490</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>24.1295774647887</v>
+        <v>24.1880341880342</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B5">
-        <v>8600</v>
+        <v>8460</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>24.1573033707865</v>
+        <v>24.1025641025641</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B6">
-        <v>8540</v>
+        <v>8439</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>24.1926345609065</v>
+        <v>24.1114285714286</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B7">
-        <v>8490</v>
+        <v>8300</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>24.1880341880342</v>
+        <v>24.1279069767442</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="B8">
-        <v>8460</v>
+        <v>8250</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>24.1025641025641</v>
+        <v>24.2647058823529</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B9">
-        <v>8439</v>
+        <v>8220</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>24.1114285714286</v>
+        <v>24.1764705882353</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B10">
-        <v>8300</v>
+        <v>8170</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>24.1279069767442</v>
+        <v>24.1002949852507</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="B11">
-        <v>8250</v>
+        <v>8040</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>24.2647058823529</v>
+        <v>24.1441441441441</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B12">
-        <v>8220</v>
+        <v>8000</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>24.1764705882353</v>
+        <v>24.0963855421687</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B13">
-        <v>8170</v>
+        <v>7970</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>24.1002949852507</v>
+        <v>24.0785498489426</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B14">
-        <v>8040</v>
+        <v>7947</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>24.1441441441441</v>
+        <v>24.0818181818182</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B15">
-        <v>8000</v>
+        <v>7920</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>24.0963855421687</v>
+        <v>24.0729483282675</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B16">
-        <v>7970</v>
+        <v>7880</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>24.0785498489426</v>
+        <v>24.1717791411043</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B17">
-        <v>7947</v>
+        <v>7700</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>24.0818181818182</v>
+        <v>23.98753894081</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B18">
-        <v>7920</v>
+        <v>7676</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>24.0729483282675</v>
+        <v>23.9875</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B19">
-        <v>7880</v>
+        <v>7541</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>24.1717791411043</v>
+        <v>24.1698717948718</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B20">
-        <v>7700</v>
+        <v>7522</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>23.98753894081</v>
+        <v>23.9554140127389</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B21">
-        <v>7676</v>
+        <v>7470</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>23.9875</v>
+        <v>24.0192926045016</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B22">
-        <v>7541</v>
+        <v>7426</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>24.1698717948718</v>
+        <v>24.0323624595469</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B23">
-        <v>7522</v>
+        <v>7389</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>23.9554140127389</v>
+        <v>23.9902597402597</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B24">
-        <v>7470</v>
+        <v>7350</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>24.0192926045016</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>24.0983606557377</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B25">
-        <v>7426</v>
+        <v>7020</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>24.0323624595469</v>
+        <v>23.9590443686007</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(C25:C28)</f>
+        <v>23.849817580634</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="B26">
-        <v>7389</v>
+        <v>6930</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>23.9902597402597</v>
+        <f>B26/A26</f>
+        <v>23.8144329896907</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="B27">
-        <v>7350</v>
+        <v>6870</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>24.0983606557377</v>
+        <f>B27/A27</f>
+        <v>23.7716262975779</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B28">
-        <v>7020</v>
+        <v>6870</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>23.9590443686007</v>
+        <f>B28/A28</f>
+        <v>23.8541666666667</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>850</v>
+        <v>186</v>
       </c>
       <c r="B29">
-        <v>4420</v>
+        <v>4053</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <f>B29/A29</f>
+        <v>21.7903225806452</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
-        <v>848</v>
+        <v>164</v>
       </c>
       <c r="B30">
-        <v>4410</v>
+        <v>3504</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
-        <v>5.20047169811321</v>
+        <f>B30/A30</f>
+        <v>21.3658536585366</v>
+      </c>
+      <c r="D30">
+        <f>AVERAGE(C30:C33)</f>
+        <v>21.3447827717271</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>853</v>
+        <v>162</v>
       </c>
       <c r="B31">
-        <v>4395</v>
+        <v>3465</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
-        <v>5.15240328253224</v>
+        <f>B31/A31</f>
+        <v>21.3888888888889</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>841</v>
+        <v>162</v>
       </c>
       <c r="B32">
-        <v>4380</v>
+        <v>3441</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>5.20808561236623</v>
+        <f>B32/A32</f>
+        <v>21.2407407407407</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>839</v>
+        <v>159</v>
       </c>
       <c r="B33">
-        <v>4370</v>
+        <v>3400</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>5.20858164481526</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <f>B33/A33</f>
+        <v>21.3836477987421</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
-        <v>838</v>
+        <v>160</v>
       </c>
       <c r="B34">
-        <v>4355</v>
+        <v>3380</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C61" si="1">B34/A34</f>
-        <v>5.19689737470167</v>
+        <f t="shared" ref="C34:C63" si="1">B34/A34</f>
+        <v>21.125</v>
+      </c>
+      <c r="D34">
+        <f>AVERAGE(C34:C39)</f>
+        <v>21.0693287090063</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>838</v>
+        <v>158</v>
       </c>
       <c r="B35">
-        <v>4340</v>
+        <v>3347</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>5.17899761336515</v>
+        <v>21.1835443037975</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>836</v>
+        <v>158</v>
       </c>
       <c r="B36">
-        <v>4325</v>
+        <v>3333</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>5.17344497607655</v>
+        <v>21.0949367088608</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>837</v>
+        <v>157</v>
       </c>
       <c r="B37">
-        <v>4315</v>
+        <v>3300</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>5.15531660692951</v>
+        <v>21.0191082802548</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>839</v>
+        <v>156</v>
       </c>
       <c r="B38">
-        <v>4300</v>
+        <v>3280</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>5.12514898688915</v>
+        <v>21.025641025641</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>844</v>
+        <v>155</v>
       </c>
       <c r="B39">
-        <v>4295</v>
+        <v>3250</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>5.08886255924171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>20.9677419354839</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
-        <v>842</v>
+        <v>154</v>
       </c>
       <c r="B40">
-        <v>4270</v>
+        <v>3210</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>5.07125890736342</v>
+        <v>20.8441558441558</v>
+      </c>
+      <c r="D40">
+        <f>AVERAGE(C40:C48)</f>
+        <v>20.7773763099055</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>839</v>
+        <v>153</v>
       </c>
       <c r="B41">
-        <v>4265</v>
+        <v>3190</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>5.0834326579261</v>
+        <v>20.8496732026144</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>857</v>
+        <v>152</v>
       </c>
       <c r="B42">
-        <v>4260</v>
+        <v>3160</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>4.9708284714119</v>
+        <v>20.7894736842105</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>840</v>
+        <v>151</v>
       </c>
       <c r="B43">
-        <v>4250</v>
+        <v>3140</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>5.05952380952381</v>
+        <v>20.794701986755</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>830</v>
+        <v>150</v>
       </c>
       <c r="B44">
-        <v>4240</v>
+        <v>3100</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>5.10843373493976</v>
+        <v>20.6666666666667</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>830</v>
+        <v>149</v>
       </c>
       <c r="B45">
-        <v>4230</v>
+        <v>3090</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>5.09638554216868</v>
+        <v>20.738255033557</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>832</v>
+        <v>148</v>
       </c>
       <c r="B46">
-        <v>4210</v>
+        <v>3070</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>5.06009615384615</v>
+        <v>20.7432432432432</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>829</v>
+        <v>147</v>
       </c>
       <c r="B47">
-        <v>4200</v>
+        <v>3050</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>5.06634499396864</v>
+        <v>20.7482993197279</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>827</v>
+        <v>146</v>
       </c>
       <c r="B48">
-        <v>4185</v>
+        <v>3040</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>5.06045949214027</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>20.8219178082192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
-        <v>836</v>
+        <v>145</v>
       </c>
       <c r="B49">
-        <v>4165</v>
+        <v>3000</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>4.98205741626794</v>
+        <v>20.6896551724138</v>
+      </c>
+      <c r="D49">
+        <f>AVERAGE(C49:C55)</f>
+        <v>20.4422728778117</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>842</v>
+        <v>144</v>
       </c>
       <c r="B50">
-        <v>4160</v>
+        <v>2962</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>4.94061757719715</v>
+        <v>20.5694444444444</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>840</v>
+        <v>142</v>
       </c>
       <c r="B51">
-        <v>4150</v>
+        <v>2877</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>4.94047619047619</v>
+        <v>20.2605633802817</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>834</v>
+        <v>140</v>
       </c>
       <c r="B52">
-        <v>4145</v>
+        <v>2879</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>4.97002398081535</v>
+        <v>20.5642857142857</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>839</v>
+        <v>140</v>
       </c>
       <c r="B53">
-        <v>4135</v>
+        <v>2850</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>4.9284862932062</v>
+        <v>20.3571428571429</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>841</v>
+        <v>138</v>
       </c>
       <c r="B54">
-        <v>4125</v>
+        <v>2800</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>4.90487514863258</v>
+        <v>20.2898550724638</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>828</v>
+        <v>137</v>
       </c>
       <c r="B55">
-        <v>4120</v>
+        <v>2790</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>4.97584541062802</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>20.3649635036496</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="B56">
-        <v>4060</v>
+        <v>2740</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>22.0652173913043</v>
+        <v>20.1470588235294</v>
+      </c>
+      <c r="D56">
+        <f>AVERAGE(C56:C58)</f>
+        <v>20.0241439859526</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B57">
-        <v>4050</v>
+        <v>2700</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>22.0108695652174</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B58">
-        <v>4040</v>
+        <v>2670</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>22.0765027322404</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>19.9253731343284</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="B59">
-        <v>4020</v>
+        <v>2630</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>22.2099447513812</v>
+        <v>19.7744360902256</v>
+      </c>
+      <c r="D59">
+        <f>AVERAGE(C59:C62)</f>
+        <v>19.7145924920131</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="B60">
-        <v>4004</v>
+        <v>2600</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>22.2444444444444</v>
+        <v>19.6969696969697</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="B61">
-        <v>4000</v>
+        <v>2580</v>
       </c>
       <c r="C61">
-        <f t="shared" si="1"/>
-        <v>22.2222222222222</v>
+        <f t="shared" ref="C61:C84" si="2">B61/A61</f>
+        <v>19.6946564885496</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>130</v>
+      </c>
+      <c r="B62">
+        <v>2560</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>19.6923076923077</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>128</v>
+      </c>
+      <c r="B63">
+        <v>2500</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>19.53125</v>
+      </c>
+      <c r="D63">
+        <f>AVERAGE(C63:C68)</f>
+        <v>19.5430102178705</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>126</v>
+      </c>
+      <c r="B64">
+        <v>2480</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>19.6825396825397</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>125</v>
+      </c>
+      <c r="B65">
+        <v>2455</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="2"/>
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>123</v>
+      </c>
+      <c r="B66">
+        <v>2400</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="2"/>
+        <v>19.5121951219512</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>122</v>
+      </c>
+      <c r="B67">
+        <v>2376</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="2"/>
+        <v>19.4754098360656</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>120</v>
+      </c>
+      <c r="B68">
+        <v>2330</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="2"/>
+        <v>19.4166666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>120</v>
+      </c>
+      <c r="B69">
+        <v>2300</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="2"/>
+        <v>19.1666666666667</v>
+      </c>
+      <c r="D69">
+        <f>AVERAGE(C69:C73)</f>
+        <v>19.0579253691916</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>119</v>
+      </c>
+      <c r="B70">
+        <v>2296</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>19.2941176470588</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>118</v>
+      </c>
+      <c r="B71">
+        <v>2251</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="2"/>
+        <v>19.0762711864407</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>118</v>
+      </c>
+      <c r="B72">
+        <v>2236</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="2"/>
+        <v>18.9491525423729</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>117</v>
+      </c>
+      <c r="B73">
+        <v>2200</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="2"/>
+        <v>18.8034188034188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>116</v>
+      </c>
+      <c r="B74">
+        <v>2154</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>18.5689655172414</v>
+      </c>
+      <c r="D74">
+        <f>AVERAGE(C74:C78)</f>
+        <v>18.5955742483595</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>115</v>
+      </c>
+      <c r="B75">
+        <v>2150</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>18.695652173913</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>113</v>
+      </c>
+      <c r="B76">
+        <v>2100</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>18.5840707964602</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>112</v>
+      </c>
+      <c r="B77">
+        <v>2090</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>18.6607142857143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>111</v>
+      </c>
+      <c r="B78">
+        <v>2050</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="2"/>
+        <v>18.4684684684685</v>
+      </c>
+      <c r="D78">
+        <f>AVERAGE(C78:C84)</f>
+        <v>18.3032209186456</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>110</v>
+      </c>
+      <c r="B79">
+        <v>2020</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="2"/>
+        <v>18.3636363636364</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>109</v>
+      </c>
+      <c r="B80">
+        <v>2000</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="2"/>
+        <v>18.348623853211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>108</v>
+      </c>
+      <c r="B81">
+        <v>1970</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="2"/>
+        <v>18.2407407407407</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>107</v>
+      </c>
+      <c r="B82">
+        <v>1950</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="2"/>
+        <v>18.2242990654206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>106</v>
+      </c>
+      <c r="B83">
+        <v>1930</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="2"/>
+        <v>18.2075471698113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>104</v>
+      </c>
+      <c r="B84">
+        <v>1900</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="2"/>
+        <v>18.2692307692308</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>105</v>
+      </c>
+      <c r="B85">
+        <v>1880</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ref="C85:C126" si="3">B85/A85</f>
+        <v>17.9047619047619</v>
+      </c>
+      <c r="D85">
+        <f>AVERAGE(C85:C89)</f>
+        <v>17.8798947674812</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>103</v>
+      </c>
+      <c r="B86">
+        <v>1850</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="3"/>
+        <v>17.9611650485437</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>102</v>
+      </c>
+      <c r="B87">
+        <v>1827</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="3"/>
+        <v>17.9117647058824</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>101</v>
+      </c>
+      <c r="B88">
+        <v>1800</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="3"/>
+        <v>17.8217821782178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>1780</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="3"/>
+        <v>17.8</v>
+      </c>
+      <c r="D89">
+        <f>AVERAGE(C90:C111)</f>
+        <v>17.5684909429197</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>99</v>
+      </c>
+      <c r="B90">
+        <v>1750</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="3"/>
+        <v>17.6767676767677</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>97</v>
+      </c>
+      <c r="B91">
+        <v>1700</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="3"/>
+        <v>17.5257731958763</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>96</v>
+      </c>
+      <c r="B92">
+        <v>1690</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>17.6041666666667</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>95</v>
+      </c>
+      <c r="B93">
+        <v>1650</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="3"/>
+        <v>17.3684210526316</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>1600</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="3"/>
+        <v>17.3913043478261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>91</v>
+      </c>
+      <c r="B95">
+        <v>1591</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="3"/>
+        <v>17.4835164835165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>90</v>
+      </c>
+      <c r="B96">
+        <v>1580</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="3"/>
+        <v>17.5555555555556</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>88</v>
+      </c>
+      <c r="B97">
+        <v>1550</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="3"/>
+        <v>17.6136363636364</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>86</v>
+      </c>
+      <c r="B98">
+        <v>1520</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="3"/>
+        <v>17.6744186046512</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>85</v>
+      </c>
+      <c r="B99">
+        <v>1500</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="3"/>
+        <v>17.6470588235294</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>84</v>
+      </c>
+      <c r="B100">
+        <v>1480</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="3"/>
+        <v>17.6190476190476</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>83</v>
+      </c>
+      <c r="B101">
+        <v>1462</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="3"/>
+        <v>17.6144578313253</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>82</v>
+      </c>
+      <c r="B102">
+        <v>1440</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="3"/>
+        <v>17.5609756097561</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>80</v>
+      </c>
+      <c r="B103">
+        <v>1400</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="3"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>79</v>
+      </c>
+      <c r="B104">
+        <v>1391</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="3"/>
+        <v>17.6075949367089</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>77</v>
+      </c>
+      <c r="B105">
+        <v>1350</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="3"/>
+        <v>17.5324675324675</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>73</v>
+      </c>
+      <c r="B106">
+        <v>1277</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="3"/>
+        <v>17.4931506849315</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>71</v>
+      </c>
+      <c r="B107">
+        <v>1250</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="3"/>
+        <v>17.6056338028169</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>68</v>
+      </c>
+      <c r="B108">
+        <v>1200</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="3"/>
+        <v>17.6470588235294</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>62</v>
+      </c>
+      <c r="B109">
+        <v>1100</v>
+      </c>
+      <c r="C109">
+        <f>B109/A109</f>
+        <v>17.741935483871</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>60</v>
+      </c>
+      <c r="B110">
+        <v>1050</v>
+      </c>
+      <c r="C110">
+        <f>B110/A110</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>57</v>
+      </c>
+      <c r="B111">
+        <v>1000</v>
+      </c>
+      <c r="C111">
+        <f>B111/A111</f>
+        <v>17.5438596491228</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3">
+      <c r="B112">
+        <v>950</v>
+      </c>
+      <c r="C112" t="e">
+        <f>B112/A112</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113">
+        <v>900</v>
+      </c>
+      <c r="C113" t="e">
+        <f>B113/A113</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="B114">
+        <v>850</v>
+      </c>
+      <c r="C114" t="e">
+        <f>B114/A114</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115">
+        <v>800</v>
+      </c>
+      <c r="C115" t="e">
+        <f>B115/A115</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>190</v>
+      </c>
+      <c r="B116">
+        <v>3996</v>
+      </c>
+      <c r="C116">
+        <f>B116/A116</f>
+        <v>21.0315789473684</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>188</v>
+      </c>
+      <c r="B117">
+        <v>3965</v>
+      </c>
+      <c r="C117">
+        <f>B117/A117</f>
+        <v>21.0904255319149</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>191</v>
+      </c>
+      <c r="B118">
+        <v>4026</v>
+      </c>
+      <c r="C118">
+        <f>B118/A118</f>
+        <v>21.0785340314136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>202</v>
+      </c>
+      <c r="B119">
+        <v>4280</v>
+      </c>
+      <c r="C119">
+        <f>B119/A119</f>
+        <v>21.1881188118812</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>203</v>
+      </c>
+      <c r="B120">
+        <v>4312</v>
+      </c>
+      <c r="C120">
+        <f>B120/A120</f>
+        <v>21.2413793103448</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>205</v>
+      </c>
+      <c r="B121">
+        <v>4348</v>
+      </c>
+      <c r="C121">
+        <f>B121/A121</f>
+        <v>21.209756097561</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>207</v>
+      </c>
+      <c r="B122">
+        <v>4400</v>
+      </c>
+      <c r="C122">
+        <f>B122/A122</f>
+        <v>21.256038647343</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123">
+        <v>174</v>
+      </c>
+      <c r="B123">
+        <v>3600</v>
+      </c>
+      <c r="C123">
+        <f>B123/A123</f>
+        <v>20.6896551724138</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3">
+      <c r="C124" t="e">
+        <f>B124/A124</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3">
+      <c r="C125" t="e">
+        <f>B125/A125</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add coeff for 10A outlet
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10728" windowHeight="9192" activeTab="2"/>
+    <workbookView windowWidth="22368" windowHeight="9335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="for 10A" sheetId="2" r:id="rId2"/>
-    <sheet name="for 20A" sheetId="3" r:id="rId3"/>
+    <sheet name="for 20A v5" sheetId="3" r:id="rId3"/>
+    <sheet name="for 10A V5" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -34,11 +36,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,14 +53,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -71,10 +67,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -85,8 +88,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -102,23 +159,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,31 +175,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,21 +183,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,7 +205,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +217,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +289,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +343,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,73 +361,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,55 +379,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,6 +396,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -407,30 +419,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,6 +464,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -484,21 +496,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -516,135 +519,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -969,7 +978,7 @@
   <dimension ref="A1:J138"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2367,7 +2376,7 @@
   <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -3916,10 +3925,959 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A2:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="12.8888888888889"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>501</v>
+      </c>
+      <c r="B2">
+        <v>14000</v>
+      </c>
+      <c r="C2">
+        <f>B2/A2</f>
+        <v>27.9441117764471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3">
+        <v>13950</v>
+      </c>
+      <c r="C3">
+        <f>B3/A3</f>
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>490</v>
+      </c>
+      <c r="B4">
+        <v>13660</v>
+      </c>
+      <c r="C4">
+        <f>B4/A4</f>
+        <v>27.8775510204082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>488</v>
+      </c>
+      <c r="B5">
+        <v>13580</v>
+      </c>
+      <c r="C5">
+        <f>B5/A5</f>
+        <v>27.827868852459</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>485</v>
+      </c>
+      <c r="B6">
+        <v>13480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>481</v>
+      </c>
+      <c r="B7">
+        <v>13440</v>
+      </c>
+      <c r="C7">
+        <f>B7/A7</f>
+        <v>27.9417879417879</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>480</v>
+      </c>
+      <c r="B8">
+        <v>13390</v>
+      </c>
+      <c r="C8">
+        <f>B8/A8</f>
+        <v>27.8958333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>476</v>
+      </c>
+      <c r="B9">
+        <v>13310</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C24" si="0">B9/A9</f>
+        <v>27.9621848739496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>479</v>
+      </c>
+      <c r="B10">
+        <v>13290</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>27.7453027139875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>475</v>
+      </c>
+      <c r="B11">
+        <v>13220</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>27.8315789473684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>466</v>
+      </c>
+      <c r="B12">
+        <v>13020</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>27.9399141630901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>463</v>
+      </c>
+      <c r="B13">
+        <v>12880</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>27.8185745140389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>450</v>
+      </c>
+      <c r="B14">
+        <v>12500</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>27.7777777777778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>447</v>
+      </c>
+      <c r="B15">
+        <v>12440</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>27.8299776286353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>446</v>
+      </c>
+      <c r="B16">
+        <v>12350</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>27.6905829596413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>440</v>
+      </c>
+      <c r="B17">
+        <v>12250</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>27.8409090909091</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>439</v>
+      </c>
+      <c r="B18">
+        <v>12210</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>27.8132118451025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>434</v>
+      </c>
+      <c r="B19">
+        <v>12130</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>27.9493087557604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>430</v>
+      </c>
+      <c r="B20">
+        <v>12000</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>27.906976744186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>425</v>
+      </c>
+      <c r="B21">
+        <v>11870</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>27.9294117647059</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>427</v>
+      </c>
+      <c r="B22">
+        <v>11880</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>27.8220140515222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>412</v>
+      </c>
+      <c r="B23">
+        <v>11500</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>27.9126213592233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>409</v>
+      </c>
+      <c r="B24">
+        <v>11360</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>27.7750611246944</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>401</v>
+      </c>
+      <c r="B25">
+        <v>11220</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C35" si="1">B25/A25</f>
+        <v>27.9800498753117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>397</v>
+      </c>
+      <c r="B26">
+        <v>11100</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>27.9596977329975</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>359</v>
+      </c>
+      <c r="B27">
+        <v>10000</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>27.8551532033426</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>357</v>
+      </c>
+      <c r="B28">
+        <v>9955</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>27.8851540616247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>353</v>
+      </c>
+      <c r="B29">
+        <v>9851</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>27.9065155807365</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>342</v>
+      </c>
+      <c r="B30">
+        <v>9500</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>27.7777777777778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>327</v>
+      </c>
+      <c r="B31">
+        <v>9100</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>27.82874617737</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>322</v>
+      </c>
+      <c r="B32">
+        <v>9000</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>27.9503105590062</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>317</v>
+      </c>
+      <c r="B33">
+        <v>8800</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>27.7602523659306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>312</v>
+      </c>
+      <c r="B34">
+        <v>8650</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>27.724358974359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>305</v>
+      </c>
+      <c r="B35">
+        <v>8500</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C48" si="2">B35/A35</f>
+        <v>27.8688524590164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>302</v>
+      </c>
+      <c r="B36">
+        <v>8400</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>27.8145695364238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>289</v>
+      </c>
+      <c r="B37">
+        <v>8000</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>27.681660899654</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>282</v>
+      </c>
+      <c r="B38">
+        <v>7850</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>27.8368794326241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>277</v>
+      </c>
+      <c r="B39">
+        <v>7700</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>27.7978339350181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>272</v>
+      </c>
+      <c r="B40">
+        <v>7600</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>27.9411764705882</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>270</v>
+      </c>
+      <c r="B41">
+        <v>7500</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>27.7777777777778</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>265</v>
+      </c>
+      <c r="B42">
+        <v>7400</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>27.9245283018868</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>263</v>
+      </c>
+      <c r="B43">
+        <v>7300</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>27.7566539923954</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>258</v>
+      </c>
+      <c r="B44">
+        <v>7200</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>27.906976744186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>254</v>
+      </c>
+      <c r="B45">
+        <v>7100</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>27.9527559055118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>252</v>
+      </c>
+      <c r="B46">
+        <v>7000</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>27.7777777777778</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>244</v>
+      </c>
+      <c r="B47">
+        <v>6800</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>27.8688524590164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>239</v>
+      </c>
+      <c r="B48">
+        <v>6700</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>28.0334728033473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>236</v>
+      </c>
+      <c r="B49">
+        <v>6600</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C68" si="3">B49/A49</f>
+        <v>27.9661016949153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>233</v>
+      </c>
+      <c r="B50">
+        <v>6500</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>27.8969957081545</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>229</v>
+      </c>
+      <c r="B51">
+        <v>6400</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>27.9475982532751</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>227</v>
+      </c>
+      <c r="B52">
+        <v>6300</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>27.7533039647577</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>222</v>
+      </c>
+      <c r="B53">
+        <v>6200</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>27.9279279279279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>214</v>
+      </c>
+      <c r="B54">
+        <v>5947</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>27.7897196261682</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>212</v>
+      </c>
+      <c r="B55">
+        <v>5900</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>27.8301886792453</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>208</v>
+      </c>
+      <c r="B56">
+        <v>5800</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="3"/>
+        <v>27.8846153846154</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57">
+        <v>5700</v>
+      </c>
+      <c r="C57" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>145</v>
+      </c>
+      <c r="B63">
+        <v>3866</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="3"/>
+        <v>26.6620689655172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>142</v>
+      </c>
+      <c r="B64">
+        <v>3747</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="3"/>
+        <v>26.387323943662</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>43</v>
+      </c>
+      <c r="B65">
+        <v>1200</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="3"/>
+        <v>27.906976744186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>30</v>
+      </c>
+      <c r="B66">
+        <v>841</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="3"/>
+        <v>28.0333333333333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>26</v>
+      </c>
+      <c r="B67">
+        <v>730</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="3"/>
+        <v>28.0769230769231</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" t="e">
+        <f>B72/A72</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" t="e">
+        <f>B73/A73</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" t="e">
+        <f>B74/A74</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" t="e">
+        <f>B75/A75</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>544</v>
+      </c>
+      <c r="B76">
+        <v>14620</v>
+      </c>
+      <c r="C76">
+        <f>B76/A76</f>
+        <v>26.875</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>541</v>
+      </c>
+      <c r="B77">
+        <v>14600</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ref="C76:C83" si="4">B77/A77</f>
+        <v>26.9870609981516</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>502</v>
+      </c>
+      <c r="B79">
+        <v>13600</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="4"/>
+        <v>27.0916334661355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>498</v>
+      </c>
+      <c r="B80">
+        <v>13390</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="4"/>
+        <v>26.8875502008032</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>487</v>
+      </c>
+      <c r="B84">
+        <v>12990</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ref="C76:C90" si="5">B84/A84</f>
+        <v>26.6735112936345</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>481</v>
+      </c>
+      <c r="B85">
+        <v>12950</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="5"/>
+        <v>26.9230769230769</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>443</v>
+      </c>
+      <c r="B87">
+        <v>11870</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="5"/>
+        <v>26.7945823927765</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88">
+        <v>11820</v>
+      </c>
+      <c r="C88" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>440</v>
+      </c>
+      <c r="B89">
+        <v>11810</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="5"/>
+        <v>26.8409090909091</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90">
+        <v>11800</v>
+      </c>
+      <c r="C90" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -3929,74 +4887,62 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
-        <v>573</v>
+        <v>199</v>
       </c>
       <c r="B1">
-        <v>15460</v>
+        <v>3520</v>
       </c>
       <c r="C1">
         <f>B1/A1</f>
-        <v>26.9808027923211</v>
+        <v>17.6884422110553</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>569</v>
+        <v>199</v>
       </c>
       <c r="B2">
-        <v>15450</v>
+        <v>3477</v>
       </c>
       <c r="C2">
-        <f>B2/A2</f>
-        <v>27.1528998242531</v>
+        <f t="shared" ref="C2:C12" si="0">B2/A2</f>
+        <v>17.4723618090452</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="e">
-        <f>B3/A3</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="e">
-        <f>B4/A4</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="e">
-        <f>B5/A5</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="e">
-        <f>B6/A6</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>557</v>
-      </c>
-      <c r="B7">
-        <v>15000</v>
-      </c>
-      <c r="C7">
-        <f>B7/A7</f>
-        <v>26.9299820466786</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>556</v>
-      </c>
-      <c r="B8">
-        <v>14980</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:C29" si="0">B8/A8</f>
-        <v>26.9424460431655</v>
+    <row r="7" spans="3:3">
+      <c r="C7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="3:3">
@@ -4023,160 +4969,67 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="3:3">
-      <c r="C13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3">
-      <c r="C14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>544</v>
-      </c>
-      <c r="B15">
-        <v>14620</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>26.875</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>541</v>
-      </c>
-      <c r="B16">
-        <v>14600</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>26.9870609981516</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>502</v>
-      </c>
-      <c r="B18">
-        <v>13600</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>27.0916334661355</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>498</v>
-      </c>
-      <c r="B19">
-        <v>13390</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>26.8875502008032</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>487</v>
-      </c>
-      <c r="B23">
-        <v>12990</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>26.6735112936345</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>481</v>
-      </c>
-      <c r="B24">
-        <v>12950</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>26.9230769230769</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3">
-      <c r="C25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>443</v>
-      </c>
-      <c r="B26">
-        <v>11870</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>26.7945823927765</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27">
-        <v>11820</v>
-      </c>
-      <c r="C27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>440</v>
-      </c>
-      <c r="B28">
-        <v>11810</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>26.8409090909091</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29">
-        <v>11800</v>
-      </c>
-      <c r="C29" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="G2:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="7"/>
+  <cols>
+    <col min="7" max="7" width="17.2222222222222"/>
+    <col min="8" max="8" width="21.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="7:8">
+      <c r="G2" s="1">
+        <v>725050000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>92650000</v>
+      </c>
+    </row>
+    <row r="3" spans="7:8">
+      <c r="G3" s="1">
+        <v>278289479</v>
+      </c>
+      <c r="H3" s="1">
+        <v>11997912</v>
+      </c>
+    </row>
+    <row r="4" spans="7:8">
+      <c r="G4" s="1">
+        <v>54400000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5440000</v>
+      </c>
+    </row>
+    <row r="5" spans="7:8">
+      <c r="G5" s="1">
+        <f>SUM(G2:G4)</f>
+        <v>1057739479</v>
+      </c>
+      <c r="H5" s="2">
+        <f>SUM(H2:H4)</f>
+        <v>110087912</v>
+      </c>
+    </row>
+    <row r="7" spans="7:8">
+      <c r="G7" s="1">
+        <v>1057739479</v>
+      </c>
+      <c r="H7">
+        <v>110087912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change address for firmware update, adjust minimum value for caculation
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9335" activeTab="4"/>
+    <workbookView windowWidth="8772" windowHeight="5544" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -53,29 +53,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,8 +74,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,14 +121,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -158,8 +136,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,7 +174,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -183,14 +183,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,19 +205,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,7 +241,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,13 +259,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +289,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +301,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,13 +325,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,19 +361,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,49 +373,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,30 +396,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -472,6 +448,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -488,11 +490,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -519,130 +519,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3925,10 +3925,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C90"/>
+  <dimension ref="A2:C94"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -4477,11 +4477,11 @@
         <v>244</v>
       </c>
       <c r="B47">
-        <v>6800</v>
+        <v>6678</v>
       </c>
       <c r="C47">
         <f t="shared" si="2"/>
-        <v>27.8688524590164</v>
+        <v>27.3688524590164</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -4801,7 +4801,7 @@
         <v>12990</v>
       </c>
       <c r="C84">
-        <f t="shared" ref="C76:C90" si="5">B84/A84</f>
+        <f>B84/A84</f>
         <v>26.6735112936345</v>
       </c>
     </row>
@@ -4813,13 +4813,13 @@
         <v>12950</v>
       </c>
       <c r="C85">
-        <f t="shared" si="5"/>
+        <f>B85/A85</f>
         <v>26.9230769230769</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="e">
-        <f t="shared" si="5"/>
+        <f>B86/A86</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
         <v>11870</v>
       </c>
       <c r="C87">
-        <f t="shared" si="5"/>
+        <f>B87/A87</f>
         <v>26.7945823927765</v>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
         <v>11820</v>
       </c>
       <c r="C88" t="e">
-        <f t="shared" si="5"/>
+        <f>B88/A88</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
         <v>11810</v>
       </c>
       <c r="C89">
-        <f t="shared" si="5"/>
+        <f>B89/A89</f>
         <v>26.8409090909091</v>
       </c>
     </row>
@@ -4861,8 +4861,38 @@
         <v>11800</v>
       </c>
       <c r="C90" t="e">
-        <f t="shared" si="5"/>
+        <f>B90/A90</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" t="e">
+        <f>B91/A91</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" t="e">
+        <f>B92/A92</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" t="e">
+        <f>B93/A93</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>133</v>
+      </c>
+      <c r="B94">
+        <v>3634</v>
+      </c>
+      <c r="C94">
+        <f>B94/A94</f>
+        <v>27.3233082706767</v>
       </c>
     </row>
   </sheetData>
@@ -4874,10 +4904,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -4887,14 +4917,14 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
-        <v>199</v>
+        <v>389</v>
       </c>
       <c r="B1">
-        <v>3520</v>
+        <v>6827</v>
       </c>
       <c r="C1">
         <f>B1/A1</f>
-        <v>17.6884422110553</v>
+        <v>17.5501285347044</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4902,17 +4932,23 @@
         <v>199</v>
       </c>
       <c r="B2">
+        <v>3520</v>
+      </c>
+      <c r="C2">
+        <f>B2/A2</f>
+        <v>17.6884422110553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>199</v>
+      </c>
+      <c r="B3">
         <v>3477</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C12" si="0">B2/A2</f>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B3/A3</f>
         <v>17.4723618090452</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3">
-      <c r="C3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="3:3">
@@ -4965,6 +5001,12 @@
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -4980,7 +5022,7 @@
   <sheetPr/>
   <dimension ref="G2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change the time for detecting full charge
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8772" windowHeight="5544" activeTab="3"/>
+    <workbookView windowWidth="22368" windowHeight="9335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,11 +37,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -49,6 +49,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -79,21 +87,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,16 +144,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,16 +174,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,7 +205,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,25 +217,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,31 +229,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,6 +253,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -296,24 +266,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,13 +283,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,13 +325,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,25 +367,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,6 +396,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -438,15 +447,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -458,17 +458,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,20 +485,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -519,130 +519,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3927,8 +3927,8 @@
   <sheetPr/>
   <dimension ref="A2:C94"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -4741,7 +4741,7 @@
         <v>14600</v>
       </c>
       <c r="C77">
-        <f t="shared" ref="C76:C83" si="4">B77/A77</f>
+        <f t="shared" ref="C76:C94" si="4">B77/A77</f>
         <v>26.9870609981516</v>
       </c>
     </row>
@@ -4801,7 +4801,7 @@
         <v>12990</v>
       </c>
       <c r="C84">
-        <f>B84/A84</f>
+        <f t="shared" si="4"/>
         <v>26.6735112936345</v>
       </c>
     </row>
@@ -4813,13 +4813,13 @@
         <v>12950</v>
       </c>
       <c r="C85">
-        <f>B85/A85</f>
+        <f t="shared" si="4"/>
         <v>26.9230769230769</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="e">
-        <f>B86/A86</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
         <v>11870</v>
       </c>
       <c r="C87">
-        <f>B87/A87</f>
+        <f t="shared" si="4"/>
         <v>26.7945823927765</v>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
         <v>11820</v>
       </c>
       <c r="C88" t="e">
-        <f>B88/A88</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
         <v>11810</v>
       </c>
       <c r="C89">
-        <f>B89/A89</f>
+        <f t="shared" si="4"/>
         <v>26.8409090909091</v>
       </c>
     </row>
@@ -4861,25 +4861,25 @@
         <v>11800</v>
       </c>
       <c r="C90" t="e">
-        <f>B90/A90</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" t="e">
-        <f>B91/A91</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="e">
-        <f>B92/A92</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="e">
-        <f>B93/A93</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4891,7 +4891,7 @@
         <v>3634</v>
       </c>
       <c r="C94">
-        <f>B94/A94</f>
+        <f t="shared" si="4"/>
         <v>27.3233082706767</v>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
   <sheetPr/>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>